<commit_message>
add shareskill and signin steps
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/Test data Manage Listing.xlsx
+++ b/MarsFramework/ExcelData/Test data Manage Listing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\himal\Competition Task\Mars Framework\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE144B20-875D-4B11-9008-97DBDD935324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9D395E-06FE-4CEC-8746-E011C04993C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4630" yWindow="1730" windowWidth="14400" windowHeight="8170" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2050" yWindow="2620" windowWidth="14400" windowHeight="8170" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="1" r:id="rId1"/>
@@ -531,12 +531,12 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="1" max="1" width="28.81640625" customWidth="1"/>
     <col min="2" max="2" width="13.08984375" customWidth="1"/>
     <col min="3" max="3" width="18.36328125" customWidth="1"/>
   </cols>

</xml_diff>